<commit_message>
Limpieza repositorio y analisis datos manuales
</commit_message>
<xml_diff>
--- a/DataVerification.xlsx
+++ b/DataVerification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juannquinones/Library/CloudStorage/OneDrive-ESCUELACOLOMBIANADEINGENIERIAJULIOGARAVITO/Nico/Manos/HigieneManos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\Hands\HigieneManos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B823862-989E-7B40-AF18-8001B3399773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34705438-5C84-4E99-ABDE-A4056D492F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1240" windowWidth="27640" windowHeight="16760" xr2:uid="{ECBA4DF4-467D-5A40-8BD2-40E7E675E489}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ECBA4DF4-467D-5A40-8BD2-40E7E675E489}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>id</t>
   </si>
@@ -120,13 +120,16 @@
     <t xml:space="preserve">no hizo uno del 4 </t>
   </si>
   <si>
-    <t>3,66</t>
+    <t>falto el 3</t>
   </si>
   <si>
-    <t>no hizo el uni</t>
+    <t>no hizo el uno</t>
   </si>
   <si>
-    <t>falto el 3</t>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>1.08|1.46</t>
   </si>
 </sst>
 </file>
@@ -211,13 +214,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,15 +559,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1680CF26-0D60-BD4C-9D51-6728540ED3FB}">
-  <dimension ref="A1:O76"/>
+  <dimension ref="A1:N76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M76" sqref="M76"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -600,2726 +607,2761 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N1" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>12</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="3">
+      <c r="C2" s="6">
         <v>1.4</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="6">
         <v>1.68</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="6">
         <v>2.4500000000000002</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="6">
         <v>3.06</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="6">
         <v>4.78</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="6">
         <v>2.06</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="6">
         <v>2.1</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="6">
         <v>2.31</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="6">
         <v>1.1499999999999999</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="6">
         <v>2.2999999999999998</v>
       </c>
-      <c r="M2" s="3"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M2" s="6"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>19</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3">
+      <c r="C3" s="6">
         <v>3.4</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="6">
         <v>1.56</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="6">
         <v>0.09</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="6">
         <v>3.45</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="6">
         <v>2.4900000000000002</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="6">
         <v>2.0099999999999998</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="6">
         <v>1.1599999999999999</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="6">
         <v>0.93</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3" s="6">
         <v>1.1299999999999999</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="6">
         <v>1.94</v>
       </c>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M3" s="6"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>23</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="3">
+      <c r="C4" s="6">
         <v>5.23</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="6">
         <v>1.85</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="6">
         <v>1.28</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="6">
         <v>1.43</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="6">
         <v>4.01</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="6">
         <v>2.08</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="6">
         <v>1.36</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="6">
         <v>2.0499999999999998</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="6">
         <v>2.2000000000000002</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="6">
         <v>3.65</v>
       </c>
-      <c r="M4" s="3"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>27</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="3">
+      <c r="C5" s="6">
         <v>6.11</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="6">
         <v>2.08</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="6">
         <v>1.36</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="6">
         <v>2.46</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="6">
         <v>2.31</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="6">
         <v>1.56</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="6">
         <v>3.28</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="6">
         <v>1</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="6">
         <v>1.38</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="6">
         <v>1.65</v>
       </c>
-      <c r="M5" s="3"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M5" s="6"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>29</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="3">
+      <c r="C6" s="6">
         <v>3.46</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="6">
         <v>2.0099999999999998</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="6">
         <v>2.2599999999999998</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="6">
         <v>4.03</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="6">
         <v>2.2799999999999998</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="6">
         <v>3.01</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="6">
         <v>2.06</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="6">
         <v>1.63</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="6">
         <v>2.25</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="6">
         <v>1.06</v>
       </c>
-      <c r="M6" s="3"/>
-      <c r="N6" s="4">
-        <v>1.08</v>
-      </c>
-      <c r="O6" s="4">
-        <v>1.46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M6" s="6"/>
+      <c r="N6" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>30</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="3">
+      <c r="C7" s="6">
         <v>3.64</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="6">
         <v>2</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="6">
         <v>2.4300000000000002</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="6">
         <v>2.15</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="6">
         <v>1.63</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="6">
         <v>2.88</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="6">
         <v>2.86</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="6">
         <v>2.95</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="6">
         <v>2.11</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="6">
         <v>2.33</v>
       </c>
-      <c r="M7" s="3"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M7" s="6"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>31</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="3">
+      <c r="C8" s="6">
         <v>3.43</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="6">
         <v>2.89</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="6">
         <v>3.84</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="6">
         <v>4.13</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="6">
         <v>4.6900000000000004</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="6">
         <v>2.06</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="6">
         <v>3.23</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="6">
         <v>2.68</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="6">
         <v>2.95</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8" s="6">
         <v>3.3</v>
       </c>
-      <c r="M8" s="3"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M8" s="6"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>33</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="3">
+      <c r="C9" s="6">
         <v>0.59</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="6">
         <v>1.05</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="6">
         <v>1.61</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="6">
         <v>0.71</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="6">
         <v>1.38</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="6">
         <v>1.69</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="6">
         <v>1.64</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="6">
         <v>1.38</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="6">
         <v>0.91</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="6">
         <v>3.36</v>
       </c>
-      <c r="M9" s="3"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>34</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="3">
+      <c r="C10" s="6">
         <v>0.81</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="6">
         <v>2.0499999999999998</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="6">
         <v>1.66</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="6">
         <v>2.2799999999999998</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="6">
         <v>1.74</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="6">
         <v>1.64</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="6">
         <v>1.1100000000000001</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="6">
         <v>1.03</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="6">
         <v>1.1299999999999999</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10" s="6">
         <v>1.96</v>
       </c>
-      <c r="M10" s="3"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M10" s="6"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>35</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="3">
+      <c r="C11" s="6">
         <v>7.05</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="6">
         <v>3.25</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="6">
         <v>3.42</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="6">
         <v>0</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="6">
         <v>4.2300000000000004</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="6">
         <v>3.52</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="6">
         <v>5.66</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="6">
         <v>2.98</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11" s="6">
         <v>2.5</v>
       </c>
-      <c r="L11" s="3">
+      <c r="L11" s="6">
         <v>2.4</v>
       </c>
-      <c r="M11" s="3"/>
+      <c r="M11" s="6"/>
       <c r="N11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>36</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="3">
+      <c r="C12" s="6">
         <v>2.85</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="6">
         <v>2.64</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="6">
         <v>2.44</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="6">
         <v>2.95</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="6">
         <v>2.73</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="6">
         <v>2.54</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="6">
         <v>3.06</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="6">
         <v>2.31</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="6">
         <v>2.4</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12" s="6">
         <v>2.4900000000000002</v>
       </c>
-      <c r="M12" s="3"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>37</v>
       </c>
       <c r="B13" s="3"/>
-      <c r="C13" s="3">
+      <c r="C13" s="6">
         <v>2.61</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="6">
         <v>3.58</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="6">
         <v>5.72</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="6">
         <v>2.86</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="6">
         <v>2.41</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="6">
         <v>2.39</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="6">
         <v>2.41</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="6">
         <v>1.74</v>
       </c>
-      <c r="K13" s="3">
+      <c r="K13" s="6">
         <v>0.3</v>
       </c>
-      <c r="L13" s="3">
+      <c r="L13" s="6">
         <v>3.27</v>
       </c>
-      <c r="M13" s="3"/>
+      <c r="M13" s="6"/>
       <c r="N13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>38</v>
       </c>
       <c r="B14" s="3"/>
-      <c r="C14" s="3">
+      <c r="C14" s="6">
         <v>5.22</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="6">
         <v>1.89</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="6">
         <v>1.79</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="6">
         <v>2.2799999999999998</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="6">
         <v>1.74</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="6">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="6">
         <v>1.31</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="6">
         <v>1.81</v>
       </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
       <c r="N14" t="s">
         <v>21</v>
       </c>
-      <c r="O14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>39</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="3">
+      <c r="C15" s="6">
         <v>5.59</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="6">
         <v>2.81</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="6">
         <v>2.39</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="6">
         <v>3.21</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="6">
         <v>1.51</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="6">
         <v>1.88</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="6">
         <v>1.58</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="6">
         <v>3.94</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K15" s="6">
         <v>1.24</v>
       </c>
-      <c r="L15" s="3">
+      <c r="L15" s="6">
         <v>1.23</v>
       </c>
-      <c r="M15" s="3"/>
+      <c r="M15" s="6"/>
       <c r="N15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>40</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="3">
+      <c r="C16" s="6">
         <v>6.01</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="6">
         <v>1.81</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="6">
         <v>5.74</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="6">
         <v>4.9400000000000004</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="6">
         <v>4.3899999999999997</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="6">
         <v>2.59</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="6">
         <v>2.46</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="6">
         <v>7.23</v>
       </c>
-      <c r="K16" s="3">
+      <c r="K16" s="6">
         <v>0.4</v>
       </c>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
       <c r="N16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>41</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="3">
+      <c r="C17" s="6">
         <v>3.15</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="6">
         <v>1.41</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="6">
         <v>2.36</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="6">
         <v>1.96</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="6">
         <v>1.6</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="6">
         <v>3.73</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17" s="6">
         <v>2.56</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="6">
         <v>5.3</v>
       </c>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>44</v>
       </c>
       <c r="B18" s="3"/>
-      <c r="C18" s="3">
+      <c r="C18" s="6">
         <v>1.79</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="6">
         <v>1.51</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="6">
         <v>1.29</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="6">
         <v>1.89</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="6">
         <v>1.79</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="6">
         <v>1.31</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="6">
         <v>1.21</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="6">
         <v>1.04</v>
       </c>
-      <c r="K18" s="3">
+      <c r="K18" s="6">
         <v>0.96</v>
       </c>
-      <c r="L18" s="3">
+      <c r="L18" s="6">
         <v>1.1399999999999999</v>
       </c>
-      <c r="M18" s="3"/>
+      <c r="M18" s="6"/>
       <c r="N18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>45</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="3">
+      <c r="C19" s="6">
         <v>2.21</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="6">
         <v>1.91</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="6">
         <v>1.86</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="6">
         <v>1.46</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="6">
         <v>2.16</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="6">
         <v>1.95</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19" s="6">
         <v>2.4500000000000002</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="6">
         <v>1.46</v>
       </c>
-      <c r="K19" s="3">
+      <c r="K19" s="6">
         <v>1.73</v>
       </c>
-      <c r="L19" s="3">
+      <c r="L19" s="6">
         <v>2.71</v>
       </c>
-      <c r="M19" s="3"/>
+      <c r="M19" s="6"/>
       <c r="N19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>46</v>
       </c>
       <c r="B20" s="3"/>
-      <c r="C20" s="3">
+      <c r="C20" s="6">
         <v>1.1299999999999999</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="6">
         <v>1.33</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="6">
         <v>2.4300000000000002</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="6">
         <v>1.5</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="6">
         <v>1.23</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="6">
         <v>1.3</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="6">
         <v>0.93</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="6">
         <v>1.25</v>
       </c>
-      <c r="K20" s="3">
+      <c r="K20" s="6">
         <v>1.21</v>
       </c>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
       <c r="N20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>47</v>
       </c>
       <c r="B21" s="3"/>
-      <c r="C21" s="3">
+      <c r="C21" s="6">
         <v>3.7</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="6">
         <v>2.15</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="6">
         <v>2.36</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="6">
         <v>2.16</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="6">
         <v>4.5199999999999996</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="6">
         <v>2.0099999999999998</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="6">
         <v>1.38</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="6">
         <v>2.9</v>
       </c>
-      <c r="K21" s="3">
+      <c r="K21" s="6">
         <v>3.14</v>
       </c>
-      <c r="L21" s="3">
+      <c r="L21" s="6">
         <v>2.81</v>
       </c>
-      <c r="M21" s="3"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M21" s="6"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>48</v>
       </c>
       <c r="B22" s="3"/>
-      <c r="C22" s="3">
+      <c r="C22" s="6">
         <v>2.15</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="6">
         <v>2.36</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="6">
         <v>2.08</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="6">
         <v>1.68</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="6">
         <v>2.93</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="6">
         <v>4.01</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="6">
         <v>2.81</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="6">
         <v>4.25</v>
       </c>
-      <c r="K22" s="3">
+      <c r="K22" s="6">
         <v>1.2</v>
       </c>
-      <c r="L22" s="3">
+      <c r="L22" s="6">
         <v>1.31</v>
       </c>
-      <c r="M22" s="3">
+      <c r="M22" s="6">
         <v>1.31</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>49</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="3">
+      <c r="C23" s="6">
         <v>3.71</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="6">
         <v>1.53</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="6">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="6">
         <v>2.52</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="6">
         <v>1.77</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="6">
         <v>1.66</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="6">
         <v>2.08</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="6">
         <v>3.18</v>
       </c>
-      <c r="K23" s="3">
+      <c r="K23" s="6">
         <v>3.21</v>
       </c>
-      <c r="L23" s="3">
+      <c r="L23" s="6">
         <v>1.35</v>
       </c>
-      <c r="M23" s="3"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M23" s="6"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>50</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="3">
+      <c r="C24" s="6">
         <v>4.07</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="6">
         <v>2.36</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="6">
         <v>2.9</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="6">
         <v>3.03</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="6">
         <v>2.93</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="6">
         <v>3.2</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24" s="6">
         <v>3.96</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24" s="6">
         <v>2.0499999999999998</v>
       </c>
-      <c r="K24" s="3">
+      <c r="K24" s="6">
         <v>2.33</v>
       </c>
-      <c r="L24" s="3">
+      <c r="L24" s="6">
         <v>1.02</v>
       </c>
-      <c r="M24" s="3"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M24" s="6"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>53</v>
       </c>
       <c r="B25" s="3"/>
-      <c r="C25" s="3">
+      <c r="C25" s="6">
         <v>2.58</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="6">
         <v>2.33</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="6">
         <v>0</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="6">
         <v>2.4300000000000002</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25" s="6">
         <v>2.98</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="6">
         <v>4.13</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25" s="6">
         <v>2.4900000000000002</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="6">
         <v>4.1900000000000004</v>
       </c>
-      <c r="K25" s="3">
+      <c r="K25" s="6">
         <v>2.78</v>
       </c>
-      <c r="L25" s="3">
+      <c r="L25" s="6">
         <v>4.75</v>
       </c>
-      <c r="M25" s="3"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M25" s="6"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>54</v>
       </c>
       <c r="B26" s="3"/>
-      <c r="C26" s="3">
+      <c r="C26" s="6">
         <v>0</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="6">
         <v>3.61</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="6">
         <v>2.0499999999999998</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="6">
         <v>1.28</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="6">
         <v>1.71</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="6">
         <v>1.84</v>
       </c>
-      <c r="I26" s="3">
+      <c r="I26" s="6">
         <v>1.84</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="6">
         <v>1.61</v>
       </c>
-      <c r="K26" s="3">
+      <c r="K26" s="6">
         <v>1.39</v>
       </c>
-      <c r="L26" s="3">
+      <c r="L26" s="6">
         <v>1.7</v>
       </c>
-      <c r="M26" s="3"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M26" s="6"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>56</v>
       </c>
       <c r="B27" s="3"/>
-      <c r="C27" s="3">
+      <c r="C27" s="6">
         <v>4.22</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="6">
         <v>3.33</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="6">
         <v>3.1</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="6">
         <v>4.1900000000000004</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27" s="6">
         <v>2.58</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="6">
         <v>3.58</v>
       </c>
-      <c r="I27" s="3">
+      <c r="I27" s="6">
         <v>3.76</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27" s="6">
         <v>2.34</v>
       </c>
-      <c r="K27" s="3">
+      <c r="K27" s="6">
         <v>2.38</v>
       </c>
-      <c r="L27" s="3">
+      <c r="L27" s="6">
         <v>3.13</v>
       </c>
-      <c r="M27" s="3"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M27" s="6"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>58</v>
       </c>
       <c r="B28" s="3"/>
-      <c r="C28" s="3">
+      <c r="C28" s="6">
         <v>3.89</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="6">
         <v>2.4900000000000002</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="6">
         <v>2.83</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="6">
         <v>3.29</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G28" s="6">
         <v>2.58</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="6">
         <v>2.2799999999999998</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I28" s="6">
         <v>2.64</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28" s="6">
         <v>3.81</v>
       </c>
-      <c r="K28" s="3">
+      <c r="K28" s="6">
         <v>2.0299999999999998</v>
       </c>
-      <c r="L28" s="3">
+      <c r="L28" s="6">
         <v>4.33</v>
       </c>
-      <c r="M28" s="3">
+      <c r="M28" s="6">
         <v>2.81</v>
       </c>
       <c r="N28" s="4">
         <v>1.41</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>59</v>
       </c>
       <c r="B29" s="3"/>
-      <c r="C29" s="3">
+      <c r="C29" s="6">
         <v>4.4400000000000004</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="6">
         <v>1.46</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="6">
         <v>3.36</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="6">
         <v>3.28</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29" s="6">
         <v>4.13</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29" s="6">
         <v>3.71</v>
       </c>
-      <c r="I29" s="3">
+      <c r="I29" s="6">
         <v>3.96</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29" s="6">
         <v>3.46</v>
       </c>
-      <c r="K29" s="3">
+      <c r="K29" s="6">
         <v>2.23</v>
       </c>
-      <c r="L29" s="3">
+      <c r="L29" s="6">
         <v>3.54</v>
       </c>
-      <c r="M29" s="3"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M29" s="6"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>64</v>
       </c>
       <c r="B30" s="3"/>
-      <c r="C30" s="3">
+      <c r="C30" s="6">
         <v>5.93</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="6">
         <v>2.16</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="6">
         <v>1.31</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="6">
         <v>2.2799999999999998</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G30" s="6">
         <v>1.45</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H30" s="6">
         <v>1.4</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I30" s="6">
         <v>3.3</v>
       </c>
-      <c r="J30" s="3">
+      <c r="J30" s="6">
         <v>1.61</v>
       </c>
-      <c r="K30" s="3">
+      <c r="K30" s="6">
         <v>1.35</v>
       </c>
-      <c r="L30" s="3">
+      <c r="L30" s="6">
         <v>0.71</v>
       </c>
-      <c r="M30" s="3" t="s">
+      <c r="M30" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>66</v>
       </c>
       <c r="B31" s="3"/>
-      <c r="C31" s="3">
+      <c r="C31" s="6">
         <v>4.95</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="6">
         <v>3.76</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="6">
         <v>3.58</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="6">
         <v>3.2</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G31" s="6">
         <v>4.05</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31" s="6">
         <v>3.88</v>
       </c>
-      <c r="I31" s="3">
+      <c r="I31" s="6">
         <v>5.08</v>
       </c>
-      <c r="J31" s="3">
+      <c r="J31" s="6">
         <v>3.26</v>
       </c>
-      <c r="K31" s="3">
+      <c r="K31" s="6">
         <v>5.22</v>
       </c>
-      <c r="L31" s="3">
+      <c r="L31" s="6">
         <v>4.08</v>
       </c>
-      <c r="M31" s="3"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M31" s="6"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>67</v>
       </c>
       <c r="B32" s="3"/>
-      <c r="C32" s="3">
+      <c r="C32" s="6">
         <v>3.3</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="6">
         <v>2.58</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="6">
         <v>2.0099999999999998</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32" s="6">
         <v>1.88</v>
       </c>
-      <c r="G32" s="3">
+      <c r="G32" s="6">
         <v>1.71</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H32" s="6">
         <v>1.61</v>
       </c>
-      <c r="I32" s="3">
+      <c r="I32" s="6">
         <v>1.73</v>
       </c>
-      <c r="J32" s="3">
+      <c r="J32" s="6">
         <v>1.46</v>
       </c>
-      <c r="K32" s="3">
+      <c r="K32" s="6">
         <v>2.06</v>
       </c>
-      <c r="L32" s="3">
+      <c r="L32" s="6">
         <v>1.26</v>
       </c>
-      <c r="M32" s="3"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M32" s="6"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>68</v>
       </c>
       <c r="B33" s="3"/>
-      <c r="C33" s="3">
+      <c r="C33" s="6">
         <v>10.23</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="6">
         <v>6.44</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="6">
         <v>5.47</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33" s="6">
         <v>8.82</v>
       </c>
-      <c r="G33" s="3">
+      <c r="G33" s="6">
         <v>8.6</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H33" s="6">
         <v>0</v>
       </c>
-      <c r="I33" s="3">
+      <c r="I33" s="6">
         <v>7.77</v>
       </c>
-      <c r="J33" s="3">
+      <c r="J33" s="6">
         <v>4.21</v>
       </c>
-      <c r="K33" s="3">
+      <c r="K33" s="6">
         <v>7.57</v>
       </c>
-      <c r="L33" s="3">
+      <c r="L33" s="6">
         <v>4.62</v>
       </c>
-      <c r="M33" s="3"/>
+      <c r="M33" s="6"/>
       <c r="N33" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>69</v>
       </c>
       <c r="B34" s="3"/>
-      <c r="C34" s="3">
+      <c r="C34" s="6">
         <v>3.48</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="6">
         <v>7.57</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="6">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="6">
         <v>6.23</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G34" s="6">
         <v>4.9000000000000004</v>
       </c>
-      <c r="H34" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I34" s="3">
+      <c r="H34" s="6">
+        <v>3.66</v>
+      </c>
+      <c r="I34" s="6">
         <v>5.45</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J34" s="6">
         <v>6.7</v>
       </c>
-      <c r="K34" s="3">
+      <c r="K34" s="6">
         <v>12.14</v>
       </c>
-      <c r="L34" s="3">
+      <c r="L34" s="6">
         <v>4.87</v>
       </c>
-      <c r="M34" s="3"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M34" s="6"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>70</v>
       </c>
       <c r="B35" s="3"/>
-      <c r="C35" s="3">
+      <c r="C35" s="6">
         <v>4.3</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="6">
         <v>2.33</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35" s="6">
         <v>2.65</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35" s="6">
         <v>4.83</v>
       </c>
-      <c r="G35" s="3">
+      <c r="G35" s="6">
         <v>2.95</v>
       </c>
-      <c r="H35" s="3">
+      <c r="H35" s="6">
         <v>2.85</v>
       </c>
-      <c r="I35" s="3">
+      <c r="I35" s="6">
         <v>3</v>
       </c>
-      <c r="J35" s="3">
+      <c r="J35" s="6">
         <v>3</v>
       </c>
-      <c r="K35" s="3">
+      <c r="K35" s="6">
         <v>3</v>
       </c>
-      <c r="L35" s="3">
+      <c r="L35" s="6">
         <v>2.75</v>
       </c>
-      <c r="M35" s="3"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M35" s="6"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>71</v>
       </c>
       <c r="B36" s="3"/>
-      <c r="C36" s="3">
+      <c r="C36" s="6">
         <v>4.38</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="6">
         <v>4.82</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="6">
         <v>3.52</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36" s="6">
         <v>3.7</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G36" s="6">
         <v>3.82</v>
       </c>
-      <c r="H36" s="3">
+      <c r="H36" s="6">
         <v>4.76</v>
       </c>
-      <c r="I36" s="3">
+      <c r="I36" s="6">
         <v>4.6500000000000004</v>
       </c>
-      <c r="J36" s="3">
+      <c r="J36" s="6">
         <v>5.68</v>
       </c>
-      <c r="K36" s="3">
+      <c r="K36" s="6">
         <v>3.78</v>
       </c>
-      <c r="L36" s="3">
+      <c r="L36" s="6">
         <v>3.58</v>
       </c>
-      <c r="M36" s="3"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M36" s="6"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>72</v>
       </c>
       <c r="B37" s="3"/>
-      <c r="C37" s="3">
+      <c r="C37" s="6">
         <v>0</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="6">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37" s="6">
         <v>3.4</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37" s="6">
         <v>4.32</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G37" s="6">
         <v>3.41</v>
       </c>
-      <c r="H37" s="3">
+      <c r="H37" s="6">
         <v>2.9</v>
       </c>
-      <c r="I37" s="3">
+      <c r="I37" s="6">
         <v>2.23</v>
       </c>
-      <c r="J37" s="3">
+      <c r="J37" s="6">
         <v>3.53</v>
       </c>
-      <c r="K37" s="3">
+      <c r="K37" s="6">
         <v>0</v>
       </c>
-      <c r="L37" s="3">
+      <c r="L37" s="6">
         <v>1.38</v>
       </c>
-      <c r="M37" s="3"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M37" s="6"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>73</v>
       </c>
       <c r="B38" s="3"/>
-      <c r="C38" s="3">
+      <c r="C38" s="6">
         <v>3.76</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="6">
         <v>2.21</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38" s="6">
         <v>1.68</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F38" s="6">
         <v>2.56</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G38" s="6">
         <v>2.46</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H38" s="6">
         <v>1.88</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I38" s="6">
         <v>2.23</v>
       </c>
-      <c r="J38" s="3">
+      <c r="J38" s="6">
         <v>2.73</v>
       </c>
-      <c r="K38" s="3">
+      <c r="K38" s="6">
         <v>1.98</v>
       </c>
-      <c r="L38" s="3">
+      <c r="L38" s="6">
         <v>0.8</v>
       </c>
-      <c r="M38" s="3"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M38" s="6"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>75</v>
       </c>
       <c r="B39" s="3"/>
-      <c r="C39" s="3">
+      <c r="C39" s="6">
         <v>8.09</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="6">
         <v>2.71</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39" s="6">
         <v>2.7</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F39" s="6">
         <v>6.12</v>
       </c>
-      <c r="G39" s="3">
+      <c r="G39" s="6">
         <v>1.6</v>
       </c>
-      <c r="H39" s="3">
+      <c r="H39" s="6">
         <v>1.81</v>
       </c>
-      <c r="I39" s="3">
+      <c r="I39" s="6">
         <v>1.5</v>
       </c>
-      <c r="J39" s="3">
+      <c r="J39" s="6">
         <v>1.08</v>
       </c>
-      <c r="K39" s="3">
+      <c r="K39" s="6">
         <v>0.85</v>
       </c>
-      <c r="L39" s="3">
+      <c r="L39" s="6">
         <v>1.05</v>
       </c>
-      <c r="M39" s="3"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M39" s="6"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>78</v>
       </c>
       <c r="B40" s="3"/>
-      <c r="C40" s="3">
+      <c r="C40" s="6">
         <v>3.13</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="6">
         <v>1.66</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="6">
         <v>1.96</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F40" s="6">
         <v>2.5099999999999998</v>
       </c>
-      <c r="G40" s="3">
+      <c r="G40" s="6">
         <v>2.35</v>
       </c>
-      <c r="H40" s="3">
+      <c r="H40" s="6">
         <v>1.88</v>
       </c>
-      <c r="I40" s="3">
+      <c r="I40" s="6">
         <v>2.11</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J40" s="6">
         <v>1.4</v>
       </c>
-      <c r="K40" s="3">
+      <c r="K40" s="6">
         <v>1.69</v>
       </c>
-      <c r="L40" s="3">
+      <c r="L40" s="6">
         <v>2.16</v>
       </c>
-      <c r="M40" s="3"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M40" s="6"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>80</v>
       </c>
       <c r="B41" s="3"/>
-      <c r="C41" s="3">
+      <c r="C41" s="6">
         <v>3.26</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="6">
         <v>1.9</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="6">
         <v>3.05</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F41" s="6">
         <v>0</v>
       </c>
-      <c r="G41" s="3">
+      <c r="G41" s="6">
         <v>1.49</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H41" s="6">
         <v>1.77</v>
       </c>
-      <c r="I41" s="3">
+      <c r="I41" s="6">
         <v>1.85</v>
       </c>
-      <c r="J41" s="3">
+      <c r="J41" s="6">
         <v>1.46</v>
       </c>
-      <c r="K41" s="3">
+      <c r="K41" s="6">
         <v>1.24</v>
       </c>
-      <c r="L41" s="3">
+      <c r="L41" s="6">
         <v>0.99</v>
       </c>
-      <c r="M41" s="3"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M41" s="6"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>88</v>
       </c>
       <c r="B42" s="3"/>
-      <c r="C42" s="3">
+      <c r="C42" s="6">
         <v>8.73</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="6">
         <v>4.8499999999999996</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="6">
         <v>5.38</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F42" s="6">
         <v>9.02</v>
       </c>
-      <c r="G42" s="3">
+      <c r="G42" s="6">
         <v>4.7699999999999996</v>
       </c>
-      <c r="H42" s="3">
+      <c r="H42" s="6">
         <v>7.47</v>
       </c>
-      <c r="I42" s="3">
+      <c r="I42" s="6">
         <v>5.42</v>
       </c>
-      <c r="J42" s="3">
+      <c r="J42" s="6">
         <v>5.82</v>
       </c>
-      <c r="K42" s="3">
+      <c r="K42" s="6">
         <v>4.2300000000000004</v>
       </c>
-      <c r="L42" s="3">
+      <c r="L42" s="6">
         <v>3.12</v>
       </c>
-      <c r="M42" s="3"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M42" s="6"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>89</v>
       </c>
       <c r="B43" s="3"/>
-      <c r="C43" s="3">
+      <c r="C43" s="6">
         <v>5.15</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="6">
         <v>2.2599999999999998</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="6">
         <v>3.86</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F43" s="6">
         <v>3.66</v>
       </c>
-      <c r="G43" s="3">
+      <c r="G43" s="6">
         <v>1.01</v>
       </c>
-      <c r="H43" s="3">
+      <c r="H43" s="6">
         <v>3.35</v>
       </c>
-      <c r="I43" s="3">
+      <c r="I43" s="6">
         <v>2</v>
       </c>
-      <c r="J43" s="3">
+      <c r="J43" s="6">
         <v>1.53</v>
       </c>
-      <c r="K43" s="3">
+      <c r="K43" s="6">
         <v>0.66</v>
       </c>
-      <c r="L43" s="3">
+      <c r="L43" s="6">
         <v>0.65</v>
       </c>
-      <c r="M43" s="3"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M43" s="6"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>90</v>
       </c>
       <c r="B44" s="3"/>
-      <c r="C44" s="3">
+      <c r="C44" s="6">
         <v>3.4</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="6">
         <v>1.93</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="6">
         <v>2.56</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F44" s="6">
         <v>2.8</v>
       </c>
-      <c r="G44" s="3">
+      <c r="G44" s="6">
         <v>2.0299999999999998</v>
       </c>
-      <c r="H44" s="3">
+      <c r="H44" s="6">
         <v>3</v>
       </c>
-      <c r="I44" s="3">
+      <c r="I44" s="6">
         <v>1.43</v>
       </c>
-      <c r="J44" s="3">
+      <c r="J44" s="6">
         <v>1.8</v>
       </c>
-      <c r="K44" s="3">
+      <c r="K44" s="6">
         <v>2.76</v>
       </c>
-      <c r="L44" s="3">
+      <c r="L44" s="6">
         <v>4.43</v>
       </c>
-      <c r="M44" s="3"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M44" s="6"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>92</v>
       </c>
       <c r="B45" s="3"/>
-      <c r="C45" s="3">
+      <c r="C45" s="6">
         <v>3.47</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="6">
         <v>2.8</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="6">
         <v>3.31</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F45" s="6">
         <v>4.5199999999999996</v>
       </c>
-      <c r="G45" s="3">
+      <c r="G45" s="6">
         <v>1.63</v>
       </c>
-      <c r="H45" s="3">
+      <c r="H45" s="6">
         <v>5.03</v>
       </c>
-      <c r="I45" s="3">
+      <c r="I45" s="6">
         <v>2.5099999999999998</v>
       </c>
-      <c r="J45" s="3">
+      <c r="J45" s="6">
         <v>2.9</v>
       </c>
-      <c r="K45" s="3">
+      <c r="K45" s="6">
         <v>2.68</v>
       </c>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
+      <c r="L45" s="6"/>
+      <c r="M45" s="6"/>
       <c r="N45" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>93</v>
       </c>
       <c r="B46" s="3"/>
-      <c r="C46" s="3">
+      <c r="C46" s="6">
         <v>5.23</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="6">
         <v>3.17</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46" s="6">
         <v>4.6399999999999997</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F46" s="6">
         <v>4.88</v>
       </c>
-      <c r="G46" s="3">
+      <c r="G46" s="6">
         <v>3.65</v>
       </c>
-      <c r="H46" s="3">
+      <c r="H46" s="6">
         <v>2.08</v>
       </c>
-      <c r="I46" s="3">
+      <c r="I46" s="6">
         <v>1.41</v>
       </c>
-      <c r="J46" s="3">
+      <c r="J46" s="6">
         <v>1.68</v>
       </c>
-      <c r="K46" s="3">
+      <c r="K46" s="6">
         <v>1.48</v>
       </c>
-      <c r="L46" s="3">
+      <c r="L46" s="6">
         <v>3.08</v>
       </c>
-      <c r="M46" s="3"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M46" s="6"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>94</v>
       </c>
       <c r="B47" s="3"/>
-      <c r="C47" s="3">
+      <c r="C47" s="6">
         <v>3.23</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="6">
         <v>1.4</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E47" s="6">
         <v>1.21</v>
       </c>
-      <c r="F47" s="3">
+      <c r="F47" s="6">
         <v>2.5</v>
       </c>
-      <c r="G47" s="3">
+      <c r="G47" s="6">
         <v>1.75</v>
       </c>
-      <c r="H47" s="3">
+      <c r="H47" s="6">
         <v>1.96</v>
       </c>
-      <c r="I47" s="3">
+      <c r="I47" s="6">
         <v>1.65</v>
       </c>
-      <c r="J47" s="3">
+      <c r="J47" s="6">
         <v>1.35</v>
       </c>
-      <c r="K47" s="3">
+      <c r="K47" s="6">
         <v>1.88</v>
       </c>
-      <c r="L47" s="3">
+      <c r="L47" s="6">
         <v>1.81</v>
       </c>
-      <c r="M47" s="3"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M47" s="6"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>95</v>
       </c>
       <c r="B48" s="3"/>
-      <c r="C48" s="3">
+      <c r="C48" s="6">
         <v>3.36</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="6">
         <v>1.56</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E48" s="6">
         <v>1.5</v>
       </c>
-      <c r="F48" s="3">
+      <c r="F48" s="6">
         <v>2.2200000000000002</v>
       </c>
-      <c r="G48" s="3">
+      <c r="G48" s="6">
         <v>1.3</v>
       </c>
-      <c r="H48" s="3">
+      <c r="H48" s="6">
         <v>1.26</v>
       </c>
-      <c r="I48" s="3">
+      <c r="I48" s="6">
         <v>1.71</v>
       </c>
-      <c r="J48" s="3">
+      <c r="J48" s="6">
         <v>1.1100000000000001</v>
       </c>
-      <c r="K48" s="3">
+      <c r="K48" s="6">
         <v>1.03</v>
       </c>
-      <c r="L48" s="3">
+      <c r="L48" s="6">
         <v>1.44</v>
       </c>
-      <c r="M48" s="3"/>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M48" s="6"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>99</v>
       </c>
       <c r="B49" s="3"/>
-      <c r="C49" s="3">
+      <c r="C49" s="6">
         <v>1.94</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="6">
         <v>2.82</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E49" s="6">
         <v>2.42</v>
       </c>
-      <c r="F49" s="3">
+      <c r="F49" s="6">
         <v>2.12</v>
       </c>
-      <c r="G49" s="3">
+      <c r="G49" s="6">
         <v>2.91</v>
       </c>
-      <c r="H49" s="3">
+      <c r="H49" s="6">
         <v>3.5</v>
       </c>
-      <c r="I49" s="3">
+      <c r="I49" s="6">
         <v>2.19</v>
       </c>
-      <c r="J49" s="3">
+      <c r="J49" s="6">
         <v>2.86</v>
       </c>
-      <c r="K49" s="3">
+      <c r="K49" s="6">
         <v>1.75</v>
       </c>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L49" s="6"/>
+      <c r="M49" s="6"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>101</v>
       </c>
       <c r="B50" s="3"/>
-      <c r="C50" s="3">
+      <c r="C50" s="6">
         <v>2.57</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="6">
         <v>3.41</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E50" s="6">
         <v>1.47</v>
       </c>
-      <c r="F50" s="3">
+      <c r="F50" s="6">
         <v>1.2</v>
       </c>
-      <c r="G50" s="3">
+      <c r="G50" s="6">
         <v>2.06</v>
       </c>
-      <c r="H50" s="3">
+      <c r="H50" s="6">
         <v>2.11</v>
       </c>
-      <c r="I50" s="3">
+      <c r="I50" s="6">
         <v>2.17</v>
       </c>
-      <c r="J50" s="3">
+      <c r="J50" s="6">
         <v>2.1800000000000002</v>
       </c>
-      <c r="K50" s="3">
+      <c r="K50" s="6">
         <v>2.34</v>
       </c>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
+      <c r="L50" s="6"/>
+      <c r="M50" s="6"/>
       <c r="N50" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>102</v>
       </c>
-      <c r="C51" s="4">
+      <c r="C51" s="7">
         <v>2.64</v>
       </c>
-      <c r="D51" s="4">
+      <c r="D51" s="7">
         <v>1.71</v>
       </c>
-      <c r="E51" s="4">
+      <c r="E51" s="7">
         <v>2.21</v>
       </c>
-      <c r="F51" s="4">
+      <c r="F51" s="7">
         <v>2.88</v>
       </c>
-      <c r="G51" s="4">
+      <c r="G51" s="7">
         <v>0</v>
       </c>
-      <c r="H51" s="4">
+      <c r="H51" s="7">
         <v>0</v>
       </c>
-      <c r="I51" s="4">
+      <c r="I51" s="7">
         <v>3.49</v>
       </c>
-      <c r="J51" s="4">
+      <c r="J51" s="7">
         <v>2.85</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K51" s="8"/>
+      <c r="L51" s="8"/>
+      <c r="M51" s="8"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>103</v>
       </c>
-      <c r="C52" s="4">
+      <c r="C52" s="7">
         <v>3.51</v>
       </c>
-      <c r="D52" s="4">
+      <c r="D52" s="7">
         <v>2.33</v>
       </c>
-      <c r="E52" s="4">
+      <c r="E52" s="7">
         <v>2.11</v>
       </c>
-      <c r="F52" s="4">
+      <c r="F52" s="7">
         <v>2.4</v>
       </c>
-      <c r="G52" s="4">
+      <c r="G52" s="7">
         <v>2.25</v>
       </c>
-      <c r="H52" s="4">
+      <c r="H52" s="7">
         <v>2.44</v>
       </c>
-      <c r="I52" s="4">
+      <c r="I52" s="7">
         <v>2.0099999999999998</v>
       </c>
-      <c r="J52" s="4">
+      <c r="J52" s="7">
         <v>3.17</v>
       </c>
-      <c r="K52" s="4">
+      <c r="K52" s="7">
         <v>1.84</v>
       </c>
-      <c r="L52" s="4">
+      <c r="L52" s="7">
         <v>1.34</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M52" s="8"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>104</v>
       </c>
-      <c r="C53" s="4">
+      <c r="C53" s="7">
         <v>4.38</v>
       </c>
-      <c r="D53" s="4">
+      <c r="D53" s="7">
         <v>1.57</v>
       </c>
-      <c r="E53" s="4">
+      <c r="E53" s="7">
         <v>1.29</v>
       </c>
-      <c r="F53" s="4">
+      <c r="F53" s="7">
         <v>2.06</v>
       </c>
-      <c r="G53" s="4">
+      <c r="G53" s="7">
         <v>2.84</v>
       </c>
-      <c r="H53" s="4">
+      <c r="H53" s="7">
         <v>3.71</v>
       </c>
-      <c r="I53" s="4">
+      <c r="I53" s="7">
         <v>2.59</v>
       </c>
-      <c r="J53" s="4">
+      <c r="J53" s="7">
         <v>2.14</v>
       </c>
-      <c r="K53" s="5">
+      <c r="K53" s="9">
         <v>1.53</v>
       </c>
-      <c r="L53" s="5">
+      <c r="L53" s="9">
         <v>2.31</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M53" s="8"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>105</v>
       </c>
-      <c r="C54" s="4">
+      <c r="C54" s="7">
         <v>2.4300000000000002</v>
       </c>
-      <c r="D54" s="4">
+      <c r="D54" s="7">
         <v>1.73</v>
       </c>
-      <c r="E54" s="4">
+      <c r="E54" s="7">
         <v>2.0299999999999998</v>
       </c>
-      <c r="F54" s="4">
+      <c r="F54" s="7">
         <v>1.58</v>
       </c>
-      <c r="G54" s="4">
+      <c r="G54" s="7">
         <v>1.91</v>
       </c>
-      <c r="H54" s="4">
+      <c r="H54" s="7">
         <v>1.58</v>
       </c>
-      <c r="I54" s="4">
+      <c r="I54" s="7">
         <v>2.94</v>
       </c>
-      <c r="J54" s="4">
+      <c r="J54" s="7">
         <v>2.61</v>
       </c>
-      <c r="K54" s="5">
+      <c r="K54" s="9">
         <v>3.95</v>
       </c>
-      <c r="L54" s="5">
+      <c r="L54" s="9">
         <v>1.1599999999999999</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M54" s="8"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>107</v>
       </c>
-      <c r="C55" s="4">
+      <c r="C55" s="7">
         <v>2.76</v>
       </c>
-      <c r="D55" s="4">
+      <c r="D55" s="7">
         <v>2.75</v>
       </c>
-      <c r="E55" s="4">
+      <c r="E55" s="7">
         <v>7.51</v>
       </c>
-      <c r="F55" s="4">
+      <c r="F55" s="7">
         <v>1.51</v>
       </c>
-      <c r="G55" s="4">
+      <c r="G55" s="7">
         <v>4.34</v>
       </c>
-      <c r="H55" s="4">
+      <c r="H55" s="7">
         <v>5.55</v>
       </c>
-      <c r="I55" s="4">
+      <c r="I55" s="7">
         <v>5.13</v>
       </c>
-      <c r="J55" s="4">
+      <c r="J55" s="7">
         <v>4.57</v>
       </c>
-      <c r="K55" s="5">
+      <c r="K55" s="9">
         <v>4.22</v>
       </c>
-      <c r="L55" s="5">
+      <c r="L55" s="9">
         <v>3.64</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M55" s="8"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>108</v>
       </c>
-      <c r="C56" s="4">
+      <c r="C56" s="7">
         <v>1.67</v>
       </c>
-      <c r="D56" s="4">
+      <c r="D56" s="7">
         <v>1.79</v>
       </c>
-      <c r="E56" s="4">
+      <c r="E56" s="7">
         <v>1.51</v>
       </c>
-      <c r="F56" s="4">
+      <c r="F56" s="7">
         <v>1.46</v>
       </c>
-      <c r="G56" s="4">
+      <c r="G56" s="7">
         <v>2.2200000000000002</v>
       </c>
-      <c r="H56" s="4">
+      <c r="H56" s="7">
         <v>1.77</v>
       </c>
-      <c r="I56" s="4">
+      <c r="I56" s="7">
         <v>1.92</v>
       </c>
-      <c r="J56" s="4">
+      <c r="J56" s="7">
         <v>2.5299999999999998</v>
       </c>
-      <c r="K56" s="5">
+      <c r="K56" s="9">
         <v>0</v>
       </c>
-      <c r="L56" s="5">
+      <c r="L56" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M56" s="8"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>109</v>
       </c>
-      <c r="C57" s="4">
+      <c r="C57" s="7">
         <v>2.89</v>
       </c>
-      <c r="D57" s="4">
+      <c r="D57" s="7">
         <v>0</v>
       </c>
-      <c r="E57" s="4">
+      <c r="E57" s="7">
         <v>2.83</v>
       </c>
-      <c r="F57" s="4">
+      <c r="F57" s="7">
         <v>1.84</v>
       </c>
-      <c r="G57" s="4">
+      <c r="G57" s="7">
         <v>2.44</v>
       </c>
-      <c r="H57" s="4">
+      <c r="H57" s="7">
         <v>1.53</v>
       </c>
-      <c r="I57" s="4">
+      <c r="I57" s="7">
         <v>1.48</v>
       </c>
-      <c r="J57" s="4">
+      <c r="J57" s="7">
         <v>1.1200000000000001</v>
       </c>
-      <c r="K57" s="5">
+      <c r="K57" s="9">
         <v>1.33</v>
       </c>
-      <c r="L57" s="5">
+      <c r="L57" s="9">
         <v>1.63</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M57" s="8"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>110</v>
       </c>
-      <c r="C58" s="4">
+      <c r="C58" s="7">
         <v>3.51</v>
       </c>
-      <c r="D58" s="4">
+      <c r="D58" s="7">
         <v>1.1599999999999999</v>
       </c>
-      <c r="E58" s="4">
+      <c r="E58" s="7">
         <v>4.12</v>
       </c>
-      <c r="F58" s="4">
+      <c r="F58" s="7">
         <v>3.05</v>
       </c>
-      <c r="G58" s="4">
+      <c r="G58" s="7">
         <v>2.0099999999999998</v>
       </c>
-      <c r="H58" s="4">
+      <c r="H58" s="7">
         <v>2.29</v>
       </c>
-      <c r="I58" s="4">
+      <c r="I58" s="7">
         <v>1.43</v>
       </c>
-      <c r="J58" s="4">
+      <c r="J58" s="7">
         <v>1.35</v>
       </c>
-      <c r="K58" s="5">
+      <c r="K58" s="9">
         <v>1.27</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L58" s="8"/>
+      <c r="M58" s="8"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>112</v>
       </c>
-      <c r="C59" s="4">
+      <c r="C59" s="7">
         <v>1.66</v>
       </c>
-      <c r="D59" s="4">
+      <c r="D59" s="7">
         <v>1.2</v>
       </c>
-      <c r="E59" s="4">
+      <c r="E59" s="7">
         <v>3.34</v>
       </c>
-      <c r="F59" s="4">
+      <c r="F59" s="7">
         <v>4.5199999999999996</v>
       </c>
-      <c r="G59" s="4">
+      <c r="G59" s="7">
         <v>2.99</v>
       </c>
-      <c r="H59" s="4">
+      <c r="H59" s="7">
         <v>2.25</v>
       </c>
-      <c r="I59" s="4">
+      <c r="I59" s="7">
         <v>2.86</v>
       </c>
-      <c r="J59" s="4">
+      <c r="J59" s="7">
         <v>1.37</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K59" s="8"/>
+      <c r="L59" s="8"/>
+      <c r="M59" s="8"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>113</v>
       </c>
-      <c r="C60" s="4">
+      <c r="C60" s="7">
         <v>4.67</v>
       </c>
-      <c r="D60" s="4">
+      <c r="D60" s="7">
         <v>3.23</v>
       </c>
-      <c r="E60" s="4">
+      <c r="E60" s="7">
         <v>8.64</v>
       </c>
-      <c r="F60" s="4">
+      <c r="F60" s="7">
         <v>12.09</v>
       </c>
-      <c r="G60" s="4">
+      <c r="G60" s="7">
         <v>4.8899999999999997</v>
       </c>
-      <c r="H60" s="4">
+      <c r="H60" s="7">
         <v>4.63</v>
       </c>
-      <c r="I60" s="4">
+      <c r="I60" s="7">
         <v>5.24</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J60" s="8"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="8"/>
+      <c r="M60" s="8"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>114</v>
       </c>
-      <c r="C61" s="4">
+      <c r="C61" s="7">
         <v>3.63</v>
       </c>
-      <c r="D61" s="4">
+      <c r="D61" s="7">
         <v>3.62</v>
       </c>
-      <c r="E61" s="4">
+      <c r="E61" s="7">
         <v>2.83</v>
       </c>
-      <c r="F61" s="4">
+      <c r="F61" s="7">
         <v>2.86</v>
       </c>
-      <c r="G61" s="4">
+      <c r="G61" s="7">
         <v>4</v>
       </c>
-      <c r="H61" s="4">
+      <c r="H61" s="7">
         <v>3.03</v>
       </c>
-      <c r="I61" s="4">
+      <c r="I61" s="7">
         <v>2.66</v>
       </c>
-      <c r="J61" s="4">
+      <c r="J61" s="7">
         <v>3.39</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K61" s="8"/>
+      <c r="L61" s="8"/>
+      <c r="M61" s="8"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>115</v>
       </c>
-      <c r="C62" s="4">
+      <c r="C62" s="7">
         <v>3.18</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D62" s="7">
         <v>1.54</v>
       </c>
-      <c r="E62" s="4">
+      <c r="E62" s="7">
         <v>2.8</v>
       </c>
-      <c r="F62" s="4">
+      <c r="F62" s="7">
         <v>0</v>
       </c>
-      <c r="G62" s="4">
+      <c r="G62" s="7">
         <v>1.92</v>
       </c>
-      <c r="H62" s="4">
+      <c r="H62" s="7">
         <v>1.51</v>
       </c>
-      <c r="I62" s="4">
+      <c r="I62" s="7">
         <v>2.14</v>
       </c>
-      <c r="J62" s="5">
+      <c r="J62" s="9">
         <v>2.2290000000000001</v>
       </c>
-      <c r="K62" s="5">
+      <c r="K62" s="9">
         <v>1.61</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L62" s="8"/>
+      <c r="M62" s="8"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>116</v>
       </c>
-      <c r="C63" s="4">
+      <c r="C63" s="7">
         <v>3.01</v>
       </c>
-      <c r="D63" s="4">
+      <c r="D63" s="7">
         <v>1.69</v>
       </c>
-      <c r="E63" s="4">
+      <c r="E63" s="7">
         <v>1.75</v>
       </c>
-      <c r="F63" s="4">
+      <c r="F63" s="7">
         <v>2.1800000000000002</v>
       </c>
-      <c r="G63" s="4">
+      <c r="G63" s="7">
         <v>1.99</v>
       </c>
-      <c r="H63" s="4">
+      <c r="H63" s="7">
         <v>1.88</v>
       </c>
-      <c r="I63" s="4">
+      <c r="I63" s="7">
         <v>2.42</v>
       </c>
-      <c r="J63" s="5">
+      <c r="J63" s="9">
         <v>1.75</v>
       </c>
-      <c r="K63" s="5">
+      <c r="K63" s="9">
         <v>2.02</v>
       </c>
-      <c r="L63" s="5">
+      <c r="L63" s="9">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M63" s="8"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
         <v>118</v>
       </c>
-      <c r="C64" s="4">
+      <c r="C64" s="7">
         <v>2.81</v>
       </c>
-      <c r="D64" s="4">
+      <c r="D64" s="7">
         <v>1.63</v>
       </c>
-      <c r="E64" s="4">
+      <c r="E64" s="7">
         <v>1.43</v>
       </c>
-      <c r="F64" s="4">
+      <c r="F64" s="7">
         <v>3.13</v>
       </c>
-      <c r="G64" s="4">
+      <c r="G64" s="7">
         <v>1.69</v>
       </c>
-      <c r="H64" s="4">
+      <c r="H64" s="7">
         <v>1.53</v>
       </c>
-      <c r="I64" s="4">
+      <c r="I64" s="7">
         <v>0.98</v>
       </c>
-      <c r="J64" s="5">
+      <c r="J64" s="9">
         <v>0.93</v>
       </c>
-      <c r="K64" s="5">
+      <c r="K64" s="9">
         <v>0.98</v>
       </c>
-      <c r="L64" s="5">
+      <c r="L64" s="9">
         <v>1.76</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M64" s="8"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
         <v>119</v>
       </c>
-      <c r="C65" s="4">
+      <c r="C65" s="7">
         <v>0.84</v>
       </c>
-      <c r="D65" s="4">
+      <c r="D65" s="7">
         <v>1.63</v>
       </c>
-      <c r="E65" s="4">
+      <c r="E65" s="7">
         <v>1.8</v>
       </c>
-      <c r="F65" s="4">
+      <c r="F65" s="7">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G65" s="4">
+      <c r="G65" s="7">
         <v>2.4900000000000002</v>
       </c>
-      <c r="H65" s="4">
+      <c r="H65" s="7">
         <v>3.01</v>
       </c>
-      <c r="I65" s="4">
+      <c r="I65" s="7">
         <v>2.13</v>
       </c>
-      <c r="J65" s="5">
+      <c r="J65" s="9">
         <v>1.7</v>
       </c>
-      <c r="K65" s="5">
+      <c r="K65" s="9">
         <v>1.17</v>
       </c>
-      <c r="L65" s="5">
+      <c r="L65" s="9">
         <v>1.46</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M65" s="8"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
         <v>120</v>
       </c>
-      <c r="C66" s="4">
+      <c r="C66" s="7">
         <v>2.76</v>
       </c>
-      <c r="D66" s="4">
+      <c r="D66" s="7">
         <v>1.5</v>
       </c>
-      <c r="E66" s="4">
+      <c r="E66" s="7">
         <v>1.58</v>
       </c>
-      <c r="F66" s="4">
+      <c r="F66" s="7">
         <v>3.1</v>
       </c>
-      <c r="G66" s="4">
+      <c r="G66" s="7">
         <v>2.56</v>
       </c>
-      <c r="H66" s="4">
+      <c r="H66" s="7">
         <v>3.93</v>
       </c>
-      <c r="I66" s="4">
+      <c r="I66" s="7">
         <v>1.1299999999999999</v>
       </c>
-      <c r="J66" s="5">
+      <c r="J66" s="9">
         <v>1.63</v>
       </c>
-      <c r="K66" s="5">
+      <c r="K66" s="9">
         <v>1.33</v>
       </c>
-      <c r="L66" s="5">
+      <c r="L66" s="9">
         <v>1.61</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M66" s="8"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
         <v>121</v>
       </c>
-      <c r="C67" s="4">
+      <c r="C67" s="7">
         <v>0</v>
       </c>
-      <c r="D67" s="4">
+      <c r="D67" s="7">
         <v>0</v>
       </c>
-      <c r="E67" s="4">
+      <c r="E67" s="7">
         <v>0.83</v>
       </c>
-      <c r="F67" s="4">
+      <c r="F67" s="7">
         <v>3.54</v>
       </c>
-      <c r="G67" s="4">
+      <c r="G67" s="7">
         <v>2.11</v>
       </c>
-      <c r="H67" s="4">
+      <c r="H67" s="7">
         <v>2.63</v>
       </c>
-      <c r="I67" s="4">
+      <c r="I67" s="7">
         <v>2.46</v>
       </c>
-      <c r="J67" s="5">
+      <c r="J67" s="9">
         <v>3.46</v>
       </c>
-      <c r="K67" s="5">
+      <c r="K67" s="9">
         <v>2.0299999999999998</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L67" s="8"/>
+      <c r="M67" s="8"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="4">
         <v>124</v>
       </c>
-      <c r="C68" s="4">
+      <c r="C68" s="7">
         <v>4.09</v>
       </c>
-      <c r="D68" s="4">
+      <c r="D68" s="7">
         <v>1.81</v>
       </c>
-      <c r="E68" s="4">
+      <c r="E68" s="7">
         <v>2.21</v>
       </c>
-      <c r="F68" s="4">
+      <c r="F68" s="7">
         <v>2.54</v>
       </c>
-      <c r="G68" s="4">
+      <c r="G68" s="7">
         <v>1.96</v>
       </c>
-      <c r="H68" s="4">
+      <c r="H68" s="7">
         <v>2.34</v>
       </c>
-      <c r="I68" s="4">
+      <c r="I68" s="7">
         <v>1.68</v>
       </c>
-      <c r="J68" s="5">
+      <c r="J68" s="9">
         <v>2.94</v>
       </c>
-      <c r="K68" s="5">
+      <c r="K68" s="9">
         <v>8.1</v>
       </c>
-      <c r="L68" s="5">
+      <c r="L68" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M68" s="8"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="4">
         <v>127</v>
       </c>
-      <c r="C69" s="4">
+      <c r="C69" s="7">
         <v>4.2</v>
       </c>
-      <c r="D69" s="4">
+      <c r="D69" s="7">
         <v>1.71</v>
       </c>
-      <c r="E69" s="4">
+      <c r="E69" s="7">
         <v>1.7</v>
       </c>
-      <c r="F69" s="4">
+      <c r="F69" s="7">
         <v>2.44</v>
       </c>
-      <c r="G69" s="4">
+      <c r="G69" s="7">
         <v>1.93</v>
       </c>
-      <c r="H69" s="4">
+      <c r="H69" s="7">
         <v>5.58</v>
       </c>
-      <c r="I69" s="4">
+      <c r="I69" s="7">
         <v>2.15</v>
       </c>
-      <c r="J69" s="5">
+      <c r="J69" s="9">
         <v>1.9</v>
       </c>
-      <c r="K69" s="5">
+      <c r="K69" s="9">
         <v>2.4</v>
       </c>
-      <c r="L69" s="5">
+      <c r="L69" s="9">
         <v>1.85</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M69" s="8"/>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="4">
         <v>128</v>
       </c>
-      <c r="C70" s="4">
+      <c r="C70" s="7">
         <v>2.94</v>
       </c>
-      <c r="D70" s="4">
+      <c r="D70" s="7">
         <v>2.0299999999999998</v>
       </c>
-      <c r="E70" s="4">
+      <c r="E70" s="7">
         <v>2.33</v>
       </c>
-      <c r="F70" s="4">
+      <c r="F70" s="7">
         <v>2.46</v>
       </c>
-      <c r="G70" s="4">
+      <c r="G70" s="7">
         <v>4.2300000000000004</v>
       </c>
-      <c r="H70" s="4">
+      <c r="H70" s="7">
         <v>2.4300000000000002</v>
       </c>
-      <c r="I70" s="4">
+      <c r="I70" s="7">
         <v>1.48</v>
       </c>
-      <c r="J70" s="5">
+      <c r="J70" s="9">
         <v>2.35</v>
       </c>
-      <c r="K70" s="5">
+      <c r="K70" s="9">
         <v>1.86</v>
       </c>
-      <c r="L70" s="5">
+      <c r="L70" s="9">
         <v>1.43</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M70" s="8"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="4">
         <v>129</v>
       </c>
-      <c r="C71" s="4">
+      <c r="C71" s="7">
         <v>6.55</v>
       </c>
-      <c r="D71" s="4">
+      <c r="D71" s="7">
         <v>2.5099999999999998</v>
       </c>
-      <c r="E71" s="4">
+      <c r="E71" s="7">
         <v>3.81</v>
       </c>
-      <c r="F71" s="4">
+      <c r="F71" s="7">
         <v>2.41</v>
       </c>
-      <c r="G71" s="4">
+      <c r="G71" s="7">
         <v>1.86</v>
       </c>
-      <c r="H71" s="4">
+      <c r="H71" s="7">
         <v>2.68</v>
       </c>
-      <c r="I71" s="4">
+      <c r="I71" s="7">
         <v>1.81</v>
       </c>
-      <c r="J71" s="5">
+      <c r="J71" s="9">
         <v>1.64</v>
       </c>
-      <c r="K71" s="5">
+      <c r="K71" s="9">
         <v>2.69</v>
       </c>
-      <c r="L71" s="5">
+      <c r="L71" s="9">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M71" s="8"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="4">
         <v>130</v>
       </c>
-      <c r="C72" s="4">
+      <c r="C72" s="7">
         <v>3.32</v>
       </c>
-      <c r="D72" s="4">
+      <c r="D72" s="7">
         <v>1.84</v>
       </c>
-      <c r="E72" s="4">
+      <c r="E72" s="7">
         <v>2.4700000000000002</v>
       </c>
-      <c r="F72" s="4">
+      <c r="F72" s="7">
         <v>2.74</v>
       </c>
-      <c r="G72" s="4">
+      <c r="G72" s="7">
         <v>2.13</v>
       </c>
-      <c r="H72" s="4">
+      <c r="H72" s="7">
         <v>2.11</v>
       </c>
-      <c r="I72" s="4">
+      <c r="I72" s="7">
         <v>1.64</v>
       </c>
-      <c r="J72" s="5">
+      <c r="J72" s="9">
         <v>1.23</v>
       </c>
-      <c r="K72" s="5">
+      <c r="K72" s="9">
         <v>1.66</v>
       </c>
-      <c r="L72" s="5">
+      <c r="L72" s="9">
         <v>2.31</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M72" s="8"/>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="4">
         <v>132</v>
       </c>
-      <c r="C73" s="4">
+      <c r="C73" s="7">
         <v>2.61</v>
       </c>
-      <c r="D73" s="4">
+      <c r="D73" s="7">
         <v>2.2799999999999998</v>
       </c>
-      <c r="E73" s="4">
+      <c r="E73" s="7">
         <v>2.57</v>
       </c>
-      <c r="F73" s="4">
+      <c r="F73" s="7">
         <v>4.8600000000000003</v>
       </c>
-      <c r="G73" s="4">
+      <c r="G73" s="7">
         <v>3.66</v>
       </c>
-      <c r="H73" s="4">
+      <c r="H73" s="7">
         <v>2.58</v>
       </c>
-      <c r="I73" s="4">
+      <c r="I73" s="7">
         <v>2.79</v>
       </c>
-      <c r="J73" s="5">
+      <c r="J73" s="9">
         <v>2.77</v>
       </c>
-      <c r="K73" s="5">
+      <c r="K73" s="9">
         <v>4.1100000000000003</v>
       </c>
-      <c r="L73" s="5">
+      <c r="L73" s="9">
         <v>2.59</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M73" s="8"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="4">
         <v>133</v>
       </c>
-      <c r="C74" s="4">
+      <c r="C74" s="7">
         <v>6.21</v>
       </c>
-      <c r="D74" s="4">
+      <c r="D74" s="7">
         <v>2.33</v>
       </c>
-      <c r="E74" s="4">
+      <c r="E74" s="7">
         <v>2.11</v>
       </c>
-      <c r="F74" s="4">
+      <c r="F74" s="7">
         <v>2.41</v>
       </c>
-      <c r="G74" s="4">
+      <c r="G74" s="7">
         <v>4.58</v>
       </c>
-      <c r="H74" s="4">
+      <c r="H74" s="7">
         <v>3.65</v>
       </c>
-      <c r="I74" s="4">
+      <c r="I74" s="7">
         <v>2.56</v>
       </c>
-      <c r="J74" s="5">
+      <c r="J74" s="9">
         <v>2.27</v>
       </c>
-      <c r="K74" s="5">
+      <c r="K74" s="9">
         <v>1.89</v>
       </c>
-      <c r="L74" s="5">
+      <c r="L74" s="9">
         <v>1.39</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M74" s="8"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
         <v>134</v>
       </c>
-      <c r="C75" s="4">
+      <c r="C75" s="7">
         <v>3.02</v>
       </c>
-      <c r="D75" s="4">
+      <c r="D75" s="7">
         <v>2.04</v>
       </c>
-      <c r="E75" s="4">
+      <c r="E75" s="7">
         <v>2.0299999999999998</v>
       </c>
-      <c r="F75" s="4">
+      <c r="F75" s="7">
         <v>2.1800000000000002</v>
       </c>
-      <c r="G75" s="4">
+      <c r="G75" s="7">
         <v>1.75</v>
       </c>
-      <c r="H75" s="4">
+      <c r="H75" s="7">
         <v>1.34</v>
       </c>
-      <c r="I75" s="4">
+      <c r="I75" s="7">
         <v>1.73</v>
       </c>
-      <c r="J75" s="5">
+      <c r="J75" s="9">
         <v>1.69</v>
       </c>
-      <c r="K75" s="5">
+      <c r="K75" s="9">
         <v>2.2799999999999998</v>
       </c>
-      <c r="L75" s="5">
+      <c r="L75" s="9">
         <v>2.02</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M75" s="8"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="4">
         <v>135</v>
       </c>
-      <c r="C76" s="4">
+      <c r="C76" s="7">
         <v>4.2300000000000004</v>
       </c>
-      <c r="D76" s="4">
+      <c r="D76" s="7">
         <v>1.93</v>
       </c>
-      <c r="E76" s="4">
+      <c r="E76" s="7">
         <v>2.35</v>
       </c>
-      <c r="F76" s="4">
+      <c r="F76" s="7">
         <v>5.01</v>
       </c>
-      <c r="G76" s="4">
+      <c r="G76" s="7">
         <v>1.68</v>
       </c>
-      <c r="H76" s="4">
+      <c r="H76" s="7">
         <v>1.96</v>
       </c>
-      <c r="I76" s="4">
+      <c r="I76" s="7">
         <v>1.76</v>
       </c>
-      <c r="J76" s="5">
+      <c r="J76" s="9">
         <v>3.04</v>
       </c>
-      <c r="K76" s="5">
+      <c r="K76" s="9">
         <v>4.1100000000000003</v>
       </c>
-      <c r="L76" s="5">
+      <c r="L76" s="9">
         <v>0.49</v>
       </c>
+      <c r="M76" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3334,29 +3376,29 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>

</xml_diff>